<commit_message>
Change 3 Files - update space cooling demand, retrofit saving and pumps & fans demand
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676DF814-60D2-4B99-860B-5CA78F6D8472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B52CE5-5141-42B1-BE25-4CF95BFB9EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -71,6 +71,28 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="216">
   <si>
@@ -748,14 +770,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1086,6 +1108,11 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -1846,7 +1873,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -1858,10 +1885,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1949,7 +1977,7 @@
     </xf>
     <xf numFmtId="15" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2052,7 +2080,7 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="13" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="13" borderId="3" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2094,7 +2122,7 @@
     <xf numFmtId="1" fontId="7" fillId="17" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2109,7 +2137,7 @@
     <xf numFmtId="1" fontId="7" fillId="18" borderId="27" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2124,7 +2152,7 @@
     <xf numFmtId="1" fontId="7" fillId="17" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2140,7 +2168,7 @@
     <xf numFmtId="1" fontId="7" fillId="17" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2155,7 +2183,7 @@
     <xf numFmtId="3" fontId="3" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="19" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="19" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="18" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2183,10 +2211,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="6" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="47" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="6" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="47" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="43" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2198,8 +2226,7 @@
     <xf numFmtId="9" fontId="6" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="44" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="44" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="44" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="44" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="44" fillId="20" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2216,7 +2243,7 @@
     <xf numFmtId="9" fontId="11" fillId="15" borderId="3" xfId="14" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2226,7 +2253,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2301,16 +2328,16 @@
     <xf numFmtId="0" fontId="41" fillId="16" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="18" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="17" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="16" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2327,7 +2354,7 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="20" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
@@ -2346,13 +2373,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2364,10 +2391,10 @@
     <xf numFmtId="0" fontId="35" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="30" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2400,10 +2427,12 @@
     <xf numFmtId="0" fontId="43" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="44" fillId="20" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="10" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
     <cellStyle name="Comma 2" xfId="11" xr:uid="{0ABA8B51-FCCD-40DB-958F-AE78849A8FFE}"/>
+    <cellStyle name="Currency" xfId="15" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="4" xr:uid="{E1BCE1F9-C32B-49FB-A63B-D516C5E840D2}"/>
@@ -3969,14 +3998,14 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="192" t="s">
+      <c r="A17" s="191" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="192"/>
-      <c r="C17" s="192"/>
-      <c r="D17" s="192"/>
-      <c r="E17" s="192"/>
-      <c r="F17" s="192"/>
+      <c r="B17" s="191"/>
+      <c r="C17" s="191"/>
+      <c r="D17" s="191"/>
+      <c r="E17" s="191"/>
+      <c r="F17" s="191"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
@@ -4014,13 +4043,13 @@
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="193" t="s">
+      <c r="B20" s="192" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="193"/>
-      <c r="D20" s="193"/>
-      <c r="E20" s="193"/>
-      <c r="F20" s="193"/>
+      <c r="C20" s="192"/>
+      <c r="D20" s="192"/>
+      <c r="E20" s="192"/>
+      <c r="F20" s="192"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="14"/>
@@ -4034,13 +4063,13 @@
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="194" t="s">
+      <c r="B21" s="193" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="194"/>
-      <c r="D21" s="194"/>
-      <c r="E21" s="194"/>
-      <c r="F21" s="194"/>
+      <c r="C21" s="193"/>
+      <c r="D21" s="193"/>
+      <c r="E21" s="193"/>
+      <c r="F21" s="193"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="14"/>
@@ -4054,57 +4083,57 @@
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="194" t="s">
+      <c r="B22" s="193" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="194"/>
-      <c r="D22" s="194"/>
-      <c r="E22" s="194"/>
-      <c r="F22" s="194"/>
+      <c r="C22" s="193"/>
+      <c r="D22" s="193"/>
+      <c r="E22" s="193"/>
+      <c r="F22" s="193"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="145" t="s">
+      <c r="B23" s="144" t="s">
         <v>197</v>
       </c>
-      <c r="C23" s="145"/>
-      <c r="D23" s="145"/>
-      <c r="E23" s="145"/>
-      <c r="F23" s="145"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="144"/>
+      <c r="F23" s="144"/>
     </row>
     <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="146" t="s">
+      <c r="B24" s="145" t="s">
         <v>198</v>
       </c>
-      <c r="C24" s="146"/>
-      <c r="D24" s="146"/>
+      <c r="C24" s="145"/>
+      <c r="D24" s="145"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="195"/>
-      <c r="B25" s="195"/>
-      <c r="C25" s="195"/>
-      <c r="D25" s="195"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195"/>
+      <c r="A25" s="194"/>
+      <c r="B25" s="194"/>
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="194"/>
+      <c r="F25" s="194"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="191"/>
-      <c r="B26" s="191"/>
-      <c r="C26" s="191"/>
-      <c r="D26" s="191"/>
-      <c r="E26" s="191"/>
-      <c r="F26" s="191"/>
+      <c r="A26" s="190"/>
+      <c r="B26" s="190"/>
+      <c r="C26" s="190"/>
+      <c r="D26" s="190"/>
+      <c r="E26" s="190"/>
+      <c r="F26" s="190"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
@@ -4291,17 +4320,17 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="195" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="197"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="148"/>
-      <c r="H2" s="196" t="s">
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="197"/>
+      <c r="F2" s="147"/>
+      <c r="H2" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="198"/>
+      <c r="I2" s="197"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -4328,7 +4357,7 @@
       <c r="E3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="149"/>
+      <c r="F3" s="148"/>
       <c r="H3" s="21"/>
       <c r="I3" s="22" t="s">
         <v>37</v>
@@ -4359,7 +4388,7 @@
       <c r="E4" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="150"/>
+      <c r="F4" s="149"/>
       <c r="H4" s="27"/>
       <c r="I4" s="28" t="s">
         <v>39</v>
@@ -4390,7 +4419,7 @@
       <c r="E5" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F5" s="150"/>
+      <c r="F5" s="149"/>
       <c r="H5" s="33"/>
       <c r="I5" s="28" t="s">
         <v>40</v>
@@ -4421,7 +4450,7 @@
       <c r="E6" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="150"/>
+      <c r="F6" s="149"/>
       <c r="H6" s="34" t="s">
         <v>9</v>
       </c>
@@ -4454,7 +4483,7 @@
       <c r="E7" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="150"/>
+      <c r="F7" s="149"/>
       <c r="H7" s="36"/>
       <c r="I7" s="28" t="s">
         <v>44</v>
@@ -4485,7 +4514,7 @@
       <c r="E8" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="150"/>
+      <c r="F8" s="149"/>
       <c r="H8" s="37"/>
       <c r="I8" s="28" t="s">
         <v>86</v>
@@ -4516,7 +4545,7 @@
       <c r="E9" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="150"/>
+      <c r="F9" s="149"/>
       <c r="H9" s="38"/>
       <c r="I9" s="39" t="s">
         <v>10</v>
@@ -4535,7 +4564,7 @@
       <c r="E10" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="150"/>
+      <c r="F10" s="149"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="29" t="s">
@@ -4550,7 +4579,7 @@
       <c r="E11" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="150"/>
+      <c r="F11" s="149"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="29" t="s">
@@ -4565,7 +4594,7 @@
       <c r="E12" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="150"/>
+      <c r="F12" s="149"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="29" t="s">
@@ -4580,7 +4609,7 @@
       <c r="E13" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="150"/>
+      <c r="F13" s="149"/>
     </row>
     <row r="14" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
@@ -4595,7 +4624,7 @@
       <c r="E14" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="150"/>
+      <c r="F14" s="149"/>
     </row>
     <row r="15" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
@@ -4610,11 +4639,11 @@
       <c r="E15" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F15" s="150"/>
-      <c r="H15" s="196" t="s">
+      <c r="F15" s="149"/>
+      <c r="H15" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="198"/>
+      <c r="I15" s="197"/>
     </row>
     <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
@@ -4629,7 +4658,7 @@
       <c r="E16" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="150"/>
+      <c r="F16" s="149"/>
       <c r="H16" s="48" t="s">
         <v>15</v>
       </c>
@@ -4650,7 +4679,7 @@
       <c r="E17" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="150"/>
+      <c r="F17" s="149"/>
       <c r="H17" s="52" t="s">
         <v>53</v>
       </c>
@@ -4671,7 +4700,7 @@
       <c r="E18" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="150"/>
+      <c r="F18" s="149"/>
       <c r="H18" s="52" t="s">
         <v>17</v>
       </c>
@@ -4688,13 +4717,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="199" t="s">
+      <c r="B20" s="198" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="200"/>
-      <c r="D20" s="200"/>
-      <c r="E20" s="201"/>
-      <c r="F20" s="151"/>
+      <c r="C20" s="199"/>
+      <c r="D20" s="199"/>
+      <c r="E20" s="200"/>
+      <c r="F20" s="150"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="44" t="s">
@@ -4717,7 +4746,7 @@
       <c r="B22" s="50" t="s">
         <v>199</v>
       </c>
-      <c r="C22" s="147" t="s">
+      <c r="C22" s="146" t="s">
         <v>200</v>
       </c>
       <c r="D22" s="59">
@@ -4726,7 +4755,7 @@
       <c r="E22" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="154" t="s">
+      <c r="F22" s="153" t="s">
         <v>202</v>
       </c>
     </row>
@@ -4734,7 +4763,7 @@
       <c r="B23" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="C23" s="155" t="s">
+      <c r="C23" s="154" t="s">
         <v>182</v>
       </c>
       <c r="D23" s="59">
@@ -4743,24 +4772,24 @@
       <c r="E23" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="154" t="s">
+      <c r="F23" s="153" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="157" t="s">
+      <c r="B24" s="156" t="s">
         <v>205</v>
       </c>
-      <c r="C24" s="158" t="s">
+      <c r="C24" s="157" t="s">
         <v>212</v>
       </c>
-      <c r="D24" s="159">
+      <c r="D24" s="158">
         <v>43952</v>
       </c>
-      <c r="E24" s="160" t="s">
+      <c r="E24" s="159" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="161" t="s">
+      <c r="F24" s="160" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4777,7 +4806,7 @@
       <c r="E25" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="154" t="s">
+      <c r="F25" s="153" t="s">
         <v>202</v>
       </c>
       <c r="H25" s="58" t="s">
@@ -4797,7 +4826,7 @@
       <c r="E26" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="156" t="s">
+      <c r="F26" s="155" t="s">
         <v>202</v>
       </c>
       <c r="H26" s="5" t="s">
@@ -4805,19 +4834,19 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="157" t="s">
+      <c r="B27" s="156" t="s">
         <v>210</v>
       </c>
-      <c r="C27" s="162" t="s">
+      <c r="C27" s="161" t="s">
         <v>209</v>
       </c>
-      <c r="D27" s="159">
+      <c r="D27" s="158">
         <v>43983</v>
       </c>
-      <c r="E27" s="160" t="s">
+      <c r="E27" s="159" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="161" t="s">
+      <c r="F27" s="160" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4834,87 +4863,87 @@
       <c r="E28" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F28" s="154" t="s">
+      <c r="F28" s="153" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="150"/>
-      <c r="B29" s="150"/>
-      <c r="C29" s="150"/>
-      <c r="D29" s="150"/>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
+      <c r="A29" s="149"/>
+      <c r="B29" s="149"/>
+      <c r="C29" s="149"/>
+      <c r="D29" s="149"/>
+      <c r="E29" s="149"/>
+      <c r="F29" s="149"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="150"/>
-      <c r="B30" s="150"/>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
+      <c r="A30" s="149"/>
+      <c r="B30" s="149"/>
+      <c r="C30" s="149"/>
+      <c r="D30" s="149"/>
+      <c r="E30" s="149"/>
+      <c r="F30" s="149"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="150"/>
-      <c r="B31" s="150"/>
-      <c r="C31" s="150"/>
-      <c r="D31" s="150"/>
-      <c r="E31" s="150"/>
-      <c r="F31" s="150"/>
+      <c r="A31" s="149"/>
+      <c r="B31" s="149"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="150"/>
-      <c r="B32" s="150"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
+      <c r="A32" s="149"/>
+      <c r="B32" s="149"/>
+      <c r="C32" s="149"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="149"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="150"/>
-      <c r="B33" s="150"/>
-      <c r="C33" s="150"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="150"/>
-      <c r="F33" s="150"/>
+      <c r="A33" s="149"/>
+      <c r="B33" s="149"/>
+      <c r="C33" s="149"/>
+      <c r="D33" s="149"/>
+      <c r="E33" s="149"/>
+      <c r="F33" s="149"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="150"/>
-      <c r="B34" s="150"/>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="150"/>
+      <c r="A34" s="149"/>
+      <c r="B34" s="149"/>
+      <c r="C34" s="149"/>
+      <c r="D34" s="149"/>
+      <c r="E34" s="149"/>
+      <c r="F34" s="149"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="150"/>
-      <c r="B35" s="150"/>
-      <c r="C35" s="150"/>
-      <c r="D35" s="150"/>
-      <c r="E35" s="150"/>
-      <c r="F35" s="150"/>
+      <c r="A35" s="149"/>
+      <c r="B35" s="149"/>
+      <c r="C35" s="149"/>
+      <c r="D35" s="149"/>
+      <c r="E35" s="149"/>
+      <c r="F35" s="149"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="150"/>
-      <c r="B36" s="150"/>
-      <c r="C36" s="150"/>
-      <c r="D36" s="150"/>
-      <c r="E36" s="150"/>
-      <c r="F36" s="150"/>
+      <c r="A36" s="149"/>
+      <c r="B36" s="149"/>
+      <c r="C36" s="149"/>
+      <c r="D36" s="149"/>
+      <c r="E36" s="149"/>
+      <c r="F36" s="149"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="196" t="s">
+      <c r="B38" s="195" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="197"/>
-      <c r="D38" s="197"/>
-      <c r="E38" s="198"/>
-      <c r="F38" s="148"/>
-      <c r="H38" s="202" t="s">
+      <c r="C38" s="196"/>
+      <c r="D38" s="196"/>
+      <c r="E38" s="197"/>
+      <c r="F38" s="147"/>
+      <c r="H38" s="201" t="s">
         <v>56</v>
       </c>
-      <c r="I38" s="203"/>
+      <c r="I38" s="202"/>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="61" t="s">
@@ -4929,7 +4958,7 @@
       <c r="E39" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="149"/>
+      <c r="F39" s="148"/>
       <c r="H39" s="64" t="s">
         <v>18</v>
       </c>
@@ -4950,7 +4979,7 @@
       <c r="E40" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="153"/>
+      <c r="F40" s="152"/>
       <c r="H40" s="54"/>
       <c r="I40" s="54"/>
     </row>
@@ -4959,7 +4988,7 @@
       <c r="C41" s="54"/>
       <c r="D41" s="54"/>
       <c r="E41" s="55"/>
-      <c r="F41" s="152"/>
+      <c r="F41" s="151"/>
       <c r="H41" s="54"/>
       <c r="I41" s="54"/>
     </row>
@@ -5021,7 +5050,7 @@
   <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5119,10 +5148,10 @@
       <c r="S5" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="T5" s="204" t="s">
+      <c r="T5" s="203" t="s">
         <v>114</v>
       </c>
-      <c r="U5" s="204"/>
+      <c r="U5" s="203"/>
     </row>
     <row r="6" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
@@ -5163,7 +5192,7 @@
       <c r="N6" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="O6" s="139" t="s">
+      <c r="O6" s="138" t="s">
         <v>115</v>
       </c>
       <c r="Q6" s="84"/>
@@ -5220,7 +5249,7 @@
         <f>U7</f>
         <v>3.4901289446216035E-3</v>
       </c>
-      <c r="O7" s="140">
+      <c r="O7" s="139">
         <f>Data!U59/1000</f>
         <v>11.196414691601362</v>
       </c>
@@ -5233,7 +5262,7 @@
       <c r="S7" s="80">
         <v>1.6E-2</v>
       </c>
-      <c r="T7" s="142">
+      <c r="T7" s="141">
         <f>Data!X59</f>
         <v>0.21813305903885022</v>
       </c>
@@ -5282,11 +5311,11 @@
       </c>
       <c r="N8" s="83">
         <f t="shared" ref="N8:N12" si="4">U8</f>
-        <v>5.8180441437599775E-3</v>
-      </c>
-      <c r="O8" s="141">
+        <v>6.053757862810245E-3</v>
+      </c>
+      <c r="O8" s="140">
         <f>Data!U60/1000</f>
-        <v>15.982779351113084</v>
+        <v>17.266169771719472</v>
       </c>
       <c r="Q8" s="81" t="s">
         <v>106</v>
@@ -5297,13 +5326,13 @@
       <c r="S8" s="81">
         <v>1.6E-2</v>
       </c>
-      <c r="T8" s="143">
+      <c r="T8" s="142">
         <f>Data!X60</f>
-        <v>0.36362775898499861</v>
+        <v>0.37835986642564029</v>
       </c>
       <c r="U8" s="81">
         <f t="shared" ref="U8:U12" si="5">S8*T8</f>
-        <v>5.8180441437599775E-3</v>
+        <v>6.053757862810245E-3</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5348,7 +5377,7 @@
         <f t="shared" si="4"/>
         <v>5.4263583940724319E-3</v>
       </c>
-      <c r="O9" s="140">
+      <c r="O9" s="139">
         <f>Data!S59/1000</f>
         <v>9.6084735804205188</v>
       </c>
@@ -5361,7 +5390,7 @@
       <c r="S9" s="80">
         <v>2.69E-2</v>
       </c>
-      <c r="T9" s="142">
+      <c r="T9" s="141">
         <f>Data!V59</f>
         <v>0.20172336037443986</v>
       </c>
@@ -5410,11 +5439,11 @@
       </c>
       <c r="N10" s="83">
         <f t="shared" si="4"/>
-        <v>1.1290389448443587E-2</v>
-      </c>
-      <c r="O10" s="141">
+        <v>1.186536422684824E-2</v>
+      </c>
+      <c r="O10" s="140">
         <f>Data!S60/1000</f>
-        <v>20.5630239417189</v>
+        <v>22.294679797673528</v>
       </c>
       <c r="Q10" s="81" t="s">
         <v>107</v>
@@ -5425,13 +5454,13 @@
       <c r="S10" s="81">
         <v>2.69E-2</v>
       </c>
-      <c r="T10" s="143">
+      <c r="T10" s="142">
         <f>Data!V60</f>
-        <v>0.41971707986779133</v>
+        <v>0.44109160694603122</v>
       </c>
       <c r="U10" s="81">
         <f t="shared" si="5"/>
-        <v>1.1290389448443587E-2</v>
+        <v>1.186536422684824E-2</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5476,7 +5505,7 @@
         <f t="shared" si="4"/>
         <v>9.5809185652412903E-3</v>
       </c>
-      <c r="O11" s="140">
+      <c r="O11" s="139">
         <f>Data!T59/1000</f>
         <v>14.333869646601945</v>
       </c>
@@ -5489,7 +5518,7 @@
       <c r="S11" s="80">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="T11" s="142">
+      <c r="T11" s="141">
         <f>Data!W59</f>
         <v>0.2000191767273756</v>
       </c>
@@ -5538,11 +5567,11 @@
       </c>
       <c r="N12" s="83">
         <f t="shared" si="4"/>
-        <v>2.0465578709164201E-2</v>
-      </c>
-      <c r="O12" s="141">
+        <v>2.0987111338457227E-2</v>
+      </c>
+      <c r="O12" s="140">
         <f>Data!T60/1000</f>
-        <v>22.25938755708523</v>
+        <v>24.114356797661486</v>
       </c>
       <c r="Q12" s="81" t="s">
         <v>108</v>
@@ -5553,13 +5582,13 @@
       <c r="S12" s="81">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="T12" s="143">
+      <c r="T12" s="142">
         <f>Data!W60</f>
-        <v>0.42725634048359507</v>
+        <v>0.43814428681539097</v>
       </c>
       <c r="U12" s="81">
         <f t="shared" si="5"/>
-        <v>2.0465578709164201E-2</v>
+        <v>2.0987111338457227E-2</v>
       </c>
     </row>
     <row r="19" spans="22:26" x14ac:dyDescent="0.2">
@@ -5803,8 +5832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A6DB4B-6EBE-42F5-800F-C9AB0144B3BB}">
   <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5834,33 +5863,33 @@
   <sheetData>
     <row r="1" spans="3:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L2" s="208" t="s">
+      <c r="L2" s="207" t="s">
         <v>175</v>
       </c>
-      <c r="M2" s="209"/>
-      <c r="N2" s="210"/>
-      <c r="O2" s="208" t="s">
+      <c r="M2" s="208"/>
+      <c r="N2" s="209"/>
+      <c r="O2" s="207" t="s">
         <v>176</v>
       </c>
-      <c r="P2" s="209"/>
-      <c r="Q2" s="210"/>
-      <c r="R2" s="208" t="s">
+      <c r="P2" s="208"/>
+      <c r="Q2" s="209"/>
+      <c r="R2" s="207" t="s">
         <v>186</v>
       </c>
-      <c r="S2" s="209"/>
-      <c r="T2" s="210"/>
+      <c r="S2" s="208"/>
+      <c r="T2" s="209"/>
       <c r="AD2" s="118" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="3" spans="3:42" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="207" t="s">
+      <c r="C3" s="206" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="207"/>
-      <c r="E3" s="207"/>
-      <c r="F3" s="207"/>
-      <c r="G3" s="207"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
       <c r="L3" s="88" t="s">
         <v>165</v>
       </c>
@@ -5916,12 +5945,12 @@
       <c r="AI3" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="AM3" s="181" t="s">
+      <c r="AM3" s="180" t="s">
         <v>175</v>
       </c>
-      <c r="AN3" s="181"/>
-      <c r="AO3" s="176"/>
-      <c r="AP3" s="176"/>
+      <c r="AN3" s="180"/>
+      <c r="AO3" s="175"/>
+      <c r="AP3" s="175"/>
     </row>
     <row r="4" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="89" t="s">
@@ -5973,11 +6002,11 @@
         <f>AVERAGE(R4:T4)</f>
         <v>54.181824878333337</v>
       </c>
-      <c r="V4" s="187">
+      <c r="V4" s="186">
         <f>AVERAGE(AN5:AP5)</f>
         <v>1.383820267553892</v>
       </c>
-      <c r="W4" s="187">
+      <c r="W4" s="186">
         <f>SUM(U4*V4)</f>
         <v>74.977907399693365</v>
       </c>
@@ -6042,52 +6071,52 @@
         <f t="shared" ref="U5:U12" si="0">AVERAGE(R5:T5)</f>
         <v>90.104603265666654</v>
       </c>
-      <c r="V5" s="187">
+      <c r="V5" s="186">
         <f>AVERAGE(AN8:AP8)</f>
         <v>1</v>
       </c>
-      <c r="W5" s="187">
+      <c r="W5" s="186">
         <f t="shared" ref="W5:W12" si="1">SUM(U5*V5)</f>
         <v>90.104603265666654</v>
       </c>
-      <c r="AA5" s="165" t="s">
+      <c r="AA5" s="164" t="s">
         <v>118</v>
       </c>
-      <c r="AB5" s="183">
+      <c r="AB5" s="182">
         <f>AVERAGE(AH5:AI5)*AO5</f>
         <v>323.125</v>
       </c>
-      <c r="AC5" s="184">
+      <c r="AC5" s="183">
         <f>AF5*AP5</f>
         <v>539.15574963609902</v>
       </c>
-      <c r="AD5" s="184">
+      <c r="AD5" s="183">
         <f>AG5*AN5</f>
         <v>200</v>
       </c>
       <c r="AE5" s="5"/>
-      <c r="AF5" s="166">
+      <c r="AF5" s="165">
         <v>400</v>
       </c>
-      <c r="AG5" s="166">
+      <c r="AG5" s="165">
         <v>140</v>
       </c>
-      <c r="AH5" s="167">
+      <c r="AH5" s="166">
         <v>190</v>
       </c>
-      <c r="AI5" s="166">
+      <c r="AI5" s="165">
         <v>280</v>
       </c>
       <c r="AM5" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="AN5" s="177">
+      <c r="AN5" s="176">
         <v>1.4285714285714286</v>
       </c>
-      <c r="AO5" s="177">
+      <c r="AO5" s="176">
         <v>1.375</v>
       </c>
-      <c r="AP5" s="177">
+      <c r="AP5" s="176">
         <v>1.3478893740902476</v>
       </c>
     </row>
@@ -6141,52 +6170,52 @@
         <f t="shared" si="0"/>
         <v>115.45560966933333</v>
       </c>
-      <c r="V6" s="187">
+      <c r="V6" s="186">
         <f t="shared" ref="V6:V7" si="2">AVERAGE(AN9:AP9)</f>
         <v>1</v>
       </c>
-      <c r="W6" s="187">
+      <c r="W6" s="186">
         <f t="shared" si="1"/>
         <v>115.45560966933333</v>
       </c>
-      <c r="AA6" s="168" t="s">
+      <c r="AA6" s="167" t="s">
         <v>120</v>
       </c>
-      <c r="AB6" s="183">
+      <c r="AB6" s="182">
         <f t="shared" ref="AB6:AB19" si="3">AVERAGE(AH6:AI6)*AO6</f>
         <v>646.25</v>
       </c>
-      <c r="AC6" s="185">
+      <c r="AC6" s="184">
         <f t="shared" ref="AC6:AC19" si="4">AF6*AP6</f>
         <v>1078.311499272198</v>
       </c>
-      <c r="AD6" s="185">
+      <c r="AD6" s="184">
         <f t="shared" ref="AD6:AD19" si="5">AG6*AN6</f>
         <v>400</v>
       </c>
       <c r="AE6" s="5"/>
-      <c r="AF6" s="169">
+      <c r="AF6" s="168">
         <v>800</v>
       </c>
-      <c r="AG6" s="169">
+      <c r="AG6" s="168">
         <v>280</v>
       </c>
-      <c r="AH6" s="170">
+      <c r="AH6" s="169">
         <v>380</v>
       </c>
-      <c r="AI6" s="169">
+      <c r="AI6" s="168">
         <v>560</v>
       </c>
       <c r="AM6" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="AN6" s="177">
+      <c r="AN6" s="176">
         <v>1.4285714285714286</v>
       </c>
-      <c r="AO6" s="177">
+      <c r="AO6" s="176">
         <v>1.375</v>
       </c>
-      <c r="AP6" s="177">
+      <c r="AP6" s="176">
         <v>1.3478893740902476</v>
       </c>
     </row>
@@ -6240,52 +6269,52 @@
         <f t="shared" si="0"/>
         <v>139.59487310199998</v>
       </c>
-      <c r="V7" s="187">
+      <c r="V7" s="186">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="W7" s="187">
+      <c r="W7" s="186">
         <f t="shared" si="1"/>
         <v>139.59487310199998</v>
       </c>
-      <c r="AA7" s="168" t="s">
+      <c r="AA7" s="167" t="s">
         <v>121</v>
       </c>
-      <c r="AB7" s="183">
+      <c r="AB7" s="182">
         <f t="shared" si="3"/>
         <v>804.375</v>
       </c>
-      <c r="AC7" s="185">
+      <c r="AC7" s="184">
         <f t="shared" si="4"/>
         <v>1213.1004366812228</v>
       </c>
-      <c r="AD7" s="185">
+      <c r="AD7" s="184">
         <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="AE7" s="5"/>
-      <c r="AF7" s="169">
+      <c r="AF7" s="168">
         <v>900</v>
       </c>
-      <c r="AG7" s="169">
+      <c r="AG7" s="168">
         <v>350</v>
       </c>
-      <c r="AH7" s="170">
+      <c r="AH7" s="169">
         <v>470</v>
       </c>
-      <c r="AI7" s="169">
+      <c r="AI7" s="168">
         <v>700</v>
       </c>
       <c r="AM7" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="AN7" s="177">
+      <c r="AN7" s="176">
         <v>1.4285714285714286</v>
       </c>
-      <c r="AO7" s="177">
+      <c r="AO7" s="176">
         <v>1.375</v>
       </c>
-      <c r="AP7" s="177">
+      <c r="AP7" s="176">
         <v>1.3478893740902476</v>
       </c>
     </row>
@@ -6339,52 +6368,52 @@
         <f t="shared" si="0"/>
         <v>188.85972977266667</v>
       </c>
-      <c r="V8" s="187">
+      <c r="V8" s="186">
         <f>AVERAGE(AN11:AP11)</f>
         <v>0.6377180975298572</v>
       </c>
-      <c r="W8" s="187">
+      <c r="W8" s="186">
         <f t="shared" si="1"/>
         <v>120.43926757062792</v>
       </c>
-      <c r="AA8" s="168" t="s">
+      <c r="AA8" s="167" t="s">
         <v>122</v>
       </c>
-      <c r="AB8" s="183">
+      <c r="AB8" s="182">
         <f t="shared" si="3"/>
         <v>745</v>
       </c>
-      <c r="AC8" s="185">
+      <c r="AC8" s="184">
         <f t="shared" si="4"/>
         <v>1200</v>
       </c>
-      <c r="AD8" s="185">
+      <c r="AD8" s="184">
         <f t="shared" si="5"/>
         <v>440</v>
       </c>
       <c r="AE8" s="5"/>
-      <c r="AF8" s="171">
+      <c r="AF8" s="170">
         <v>1200</v>
       </c>
-      <c r="AG8" s="169">
+      <c r="AG8" s="168">
         <v>440</v>
       </c>
-      <c r="AH8" s="170">
+      <c r="AH8" s="169">
         <v>590</v>
       </c>
-      <c r="AI8" s="169">
+      <c r="AI8" s="168">
         <v>900</v>
       </c>
       <c r="AM8" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="AN8" s="178">
+      <c r="AN8" s="177">
         <v>1</v>
       </c>
-      <c r="AO8" s="178">
+      <c r="AO8" s="177">
         <v>1</v>
       </c>
-      <c r="AP8" s="178">
+      <c r="AP8" s="177">
         <v>1</v>
       </c>
     </row>
@@ -6441,52 +6470,52 @@
         <f t="shared" si="0"/>
         <v>260.5202750266667</v>
       </c>
-      <c r="V9" s="187">
+      <c r="V9" s="186">
         <f>AVERAGE(AN14:AP14)</f>
         <v>0.66169935385599443</v>
       </c>
-      <c r="W9" s="187">
+      <c r="W9" s="186">
         <f t="shared" si="1"/>
         <v>172.38609765153132</v>
       </c>
-      <c r="AA9" s="168" t="s">
+      <c r="AA9" s="167" t="s">
         <v>123</v>
       </c>
-      <c r="AB9" s="183">
+      <c r="AB9" s="182">
         <f t="shared" si="3"/>
         <v>950</v>
       </c>
-      <c r="AC9" s="185">
+      <c r="AC9" s="184">
         <f t="shared" si="4"/>
         <v>1500</v>
       </c>
-      <c r="AD9" s="185">
+      <c r="AD9" s="184">
         <f t="shared" si="5"/>
         <v>570</v>
       </c>
       <c r="AE9" s="5"/>
-      <c r="AF9" s="171">
+      <c r="AF9" s="170">
         <v>1500</v>
       </c>
-      <c r="AG9" s="169">
+      <c r="AG9" s="168">
         <v>570</v>
       </c>
-      <c r="AH9" s="170">
+      <c r="AH9" s="169">
         <v>800</v>
       </c>
-      <c r="AI9" s="171">
+      <c r="AI9" s="170">
         <v>1100</v>
       </c>
       <c r="AM9" s="101" t="s">
         <v>123</v>
       </c>
-      <c r="AN9" s="179">
+      <c r="AN9" s="178">
         <v>1</v>
       </c>
-      <c r="AO9" s="179">
+      <c r="AO9" s="178">
         <v>1</v>
       </c>
-      <c r="AP9" s="179">
+      <c r="AP9" s="178">
         <v>1</v>
       </c>
     </row>
@@ -6540,52 +6569,52 @@
         <f t="shared" si="0"/>
         <v>337.60044621333333</v>
       </c>
-      <c r="V10" s="187">
+      <c r="V10" s="186">
         <f>AVERAGE(AN16:AP16)</f>
         <v>0.67657105591908995</v>
       </c>
-      <c r="W10" s="187">
+      <c r="W10" s="186">
         <f t="shared" si="1"/>
         <v>228.41069037331087</v>
       </c>
-      <c r="AA10" s="168" t="s">
+      <c r="AA10" s="167" t="s">
         <v>124</v>
       </c>
-      <c r="AB10" s="183">
+      <c r="AB10" s="182">
         <f t="shared" si="3"/>
         <v>1150</v>
       </c>
-      <c r="AC10" s="185">
+      <c r="AC10" s="184">
         <f t="shared" si="4"/>
         <v>1900</v>
       </c>
-      <c r="AD10" s="185">
+      <c r="AD10" s="184">
         <f t="shared" si="5"/>
         <v>700</v>
       </c>
       <c r="AE10" s="5"/>
-      <c r="AF10" s="171">
+      <c r="AF10" s="170">
         <v>1900</v>
       </c>
-      <c r="AG10" s="169">
+      <c r="AG10" s="168">
         <v>700</v>
       </c>
-      <c r="AH10" s="170">
+      <c r="AH10" s="169">
         <v>900</v>
       </c>
-      <c r="AI10" s="171">
+      <c r="AI10" s="170">
         <v>1400</v>
       </c>
       <c r="AM10" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="AN10" s="178">
+      <c r="AN10" s="177">
         <v>1</v>
       </c>
-      <c r="AO10" s="178">
+      <c r="AO10" s="177">
         <v>1</v>
       </c>
-      <c r="AP10" s="178">
+      <c r="AP10" s="177">
         <v>1</v>
       </c>
     </row>
@@ -6639,52 +6668,52 @@
         <f t="shared" si="0"/>
         <v>413.55162632333332</v>
       </c>
-      <c r="V11" s="187">
+      <c r="V11" s="186">
         <f t="shared" ref="V11:V12" si="6">AVERAGE(AN17:AP17)</f>
         <v>0.67657105591908995</v>
       </c>
-      <c r="W11" s="187">
+      <c r="W11" s="186">
         <f t="shared" si="1"/>
         <v>279.79706049863455</v>
       </c>
-      <c r="AA11" s="168" t="s">
+      <c r="AA11" s="167" t="s">
         <v>125</v>
       </c>
-      <c r="AB11" s="183">
+      <c r="AB11" s="182">
         <f t="shared" si="3"/>
         <v>862.03259827420902</v>
       </c>
-      <c r="AC11" s="185">
+      <c r="AC11" s="184">
         <f t="shared" si="4"/>
         <v>1432.4324324324325</v>
       </c>
-      <c r="AD11" s="185">
+      <c r="AD11" s="184">
         <f t="shared" si="5"/>
         <v>498.80478087649402</v>
       </c>
       <c r="AE11" s="5"/>
-      <c r="AF11" s="171">
+      <c r="AF11" s="170">
         <v>2200</v>
       </c>
-      <c r="AG11" s="169">
+      <c r="AG11" s="168">
         <v>800</v>
       </c>
-      <c r="AH11" s="172">
+      <c r="AH11" s="171">
         <v>1100</v>
       </c>
-      <c r="AI11" s="171">
+      <c r="AI11" s="170">
         <v>1600</v>
       </c>
       <c r="AM11" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="AN11" s="179">
+      <c r="AN11" s="178">
         <v>0.62350597609561753</v>
       </c>
-      <c r="AO11" s="179">
+      <c r="AO11" s="178">
         <v>0.63854266538830295</v>
       </c>
-      <c r="AP11" s="179">
+      <c r="AP11" s="178">
         <v>0.65110565110565111</v>
       </c>
     </row>
@@ -6738,50 +6767,50 @@
         <f t="shared" si="0"/>
         <v>626.50035470099999</v>
       </c>
-      <c r="V12" s="187">
+      <c r="V12" s="186">
         <f t="shared" si="6"/>
         <v>0.69007410579573669</v>
       </c>
-      <c r="W12" s="187">
+      <c r="W12" s="186">
         <f t="shared" si="1"/>
         <v>432.33167205100443</v>
       </c>
-      <c r="AA12" s="168" t="s">
+      <c r="AA12" s="167" t="s">
         <v>127</v>
       </c>
-      <c r="AB12" s="183">
+      <c r="AB12" s="182">
         <f t="shared" si="3"/>
         <v>1021.6682646212847</v>
       </c>
-      <c r="AC12" s="185">
+      <c r="AC12" s="184">
         <f t="shared" si="4"/>
         <v>1692.874692874693</v>
       </c>
-      <c r="AD12" s="185">
+      <c r="AD12" s="184">
         <f t="shared" si="5"/>
         <v>623.50597609561748</v>
       </c>
       <c r="AE12" s="5"/>
-      <c r="AF12" s="171">
+      <c r="AF12" s="170">
         <v>2600</v>
       </c>
-      <c r="AG12" s="171">
+      <c r="AG12" s="170">
         <v>1000</v>
       </c>
-      <c r="AH12" s="172">
+      <c r="AH12" s="171">
         <v>1300</v>
       </c>
-      <c r="AI12" s="171">
+      <c r="AI12" s="170">
         <v>1900</v>
       </c>
       <c r="AM12" s="101"/>
-      <c r="AN12" s="179">
+      <c r="AN12" s="178">
         <v>0.62350597609561753</v>
       </c>
-      <c r="AO12" s="179">
+      <c r="AO12" s="178">
         <v>0.63854266538830295</v>
       </c>
-      <c r="AP12" s="179">
+      <c r="AP12" s="178">
         <v>0.65110565110565111</v>
       </c>
     </row>
@@ -6810,42 +6839,42 @@
       <c r="Q13" s="113">
         <v>0.71303848954914961</v>
       </c>
-      <c r="AA13" s="168" t="s">
+      <c r="AA13" s="167" t="s">
         <v>128</v>
       </c>
-      <c r="AB13" s="183">
+      <c r="AB13" s="182">
         <f t="shared" si="3"/>
         <v>1181.3039309683604</v>
       </c>
-      <c r="AC13" s="185">
+      <c r="AC13" s="184">
         <f t="shared" si="4"/>
         <v>1888.2063882063883</v>
       </c>
-      <c r="AD13" s="185">
+      <c r="AD13" s="184">
         <f t="shared" si="5"/>
         <v>685.85657370517924</v>
       </c>
       <c r="AE13" s="5"/>
-      <c r="AF13" s="171">
+      <c r="AF13" s="170">
         <v>2900</v>
       </c>
-      <c r="AG13" s="171">
+      <c r="AG13" s="170">
         <v>1100</v>
       </c>
-      <c r="AH13" s="172">
+      <c r="AH13" s="171">
         <v>1500</v>
       </c>
-      <c r="AI13" s="171">
+      <c r="AI13" s="170">
         <v>2200</v>
       </c>
       <c r="AM13" s="101"/>
-      <c r="AN13" s="179">
+      <c r="AN13" s="178">
         <v>0.62350597609561753</v>
       </c>
-      <c r="AO13" s="179">
+      <c r="AO13" s="178">
         <v>0.63854266538830295</v>
       </c>
-      <c r="AP13" s="179">
+      <c r="AP13" s="178">
         <v>0.65110565110565111</v>
       </c>
     </row>
@@ -6868,44 +6897,44 @@
       <c r="G14" s="115">
         <v>1697580.3349999997</v>
       </c>
-      <c r="AA14" s="168" t="s">
+      <c r="AA14" s="167" t="s">
         <v>129</v>
       </c>
-      <c r="AB14" s="183">
+      <c r="AB14" s="182">
         <f t="shared" si="3"/>
         <v>1433.8643942200815</v>
       </c>
-      <c r="AC14" s="185">
+      <c r="AC14" s="184">
         <f t="shared" si="4"/>
         <v>2364.0040444893834</v>
       </c>
-      <c r="AD14" s="185">
+      <c r="AD14" s="184">
         <f t="shared" si="5"/>
         <v>835.58106169296991</v>
       </c>
       <c r="AE14" s="5"/>
-      <c r="AF14" s="171">
+      <c r="AF14" s="170">
         <v>3500</v>
       </c>
-      <c r="AG14" s="171">
+      <c r="AG14" s="170">
         <v>1300</v>
       </c>
-      <c r="AH14" s="172">
+      <c r="AH14" s="171">
         <v>1700</v>
       </c>
-      <c r="AI14" s="171">
+      <c r="AI14" s="170">
         <v>2600</v>
       </c>
       <c r="AM14" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="AN14" s="178">
+      <c r="AN14" s="177">
         <v>0.64275466284074612</v>
       </c>
-      <c r="AO14" s="178">
+      <c r="AO14" s="177">
         <v>0.6669136717302705</v>
       </c>
-      <c r="AP14" s="178">
+      <c r="AP14" s="177">
         <v>0.67542972699696668</v>
       </c>
     </row>
@@ -6913,42 +6942,42 @@
       <c r="L15" t="s">
         <v>185</v>
       </c>
-      <c r="AA15" s="168" t="s">
+      <c r="AA15" s="167" t="s">
         <v>131</v>
       </c>
-      <c r="AB15" s="183">
+      <c r="AB15" s="182">
         <f t="shared" si="3"/>
         <v>1700.6298629121898</v>
       </c>
-      <c r="AC15" s="185">
+      <c r="AC15" s="184">
         <f t="shared" si="4"/>
         <v>2769.2618806875635</v>
       </c>
-      <c r="AD15" s="185">
+      <c r="AD15" s="184">
         <f t="shared" si="5"/>
         <v>964.13199426111919</v>
       </c>
       <c r="AE15" s="5"/>
-      <c r="AF15" s="171">
+      <c r="AF15" s="170">
         <v>4100</v>
       </c>
-      <c r="AG15" s="171">
+      <c r="AG15" s="170">
         <v>1500</v>
       </c>
-      <c r="AH15" s="172">
+      <c r="AH15" s="171">
         <v>2000</v>
       </c>
-      <c r="AI15" s="171">
+      <c r="AI15" s="170">
         <v>3100</v>
       </c>
       <c r="AM15" s="96"/>
-      <c r="AN15" s="178">
+      <c r="AN15" s="177">
         <v>0.64275466284074612</v>
       </c>
-      <c r="AO15" s="178">
+      <c r="AO15" s="177">
         <v>0.6669136717302705</v>
       </c>
-      <c r="AP15" s="178">
+      <c r="AP15" s="177">
         <v>0.67542972699696668</v>
       </c>
     </row>
@@ -6959,44 +6988,44 @@
       <c r="O16" t="s">
         <v>215</v>
       </c>
-      <c r="AA16" s="168" t="s">
+      <c r="AA16" s="167" t="s">
         <v>132</v>
       </c>
-      <c r="AB16" s="183">
+      <c r="AB16" s="182">
         <f t="shared" si="3"/>
         <v>1978.8338900698452</v>
       </c>
-      <c r="AC16" s="185">
+      <c r="AC16" s="184">
         <f t="shared" si="4"/>
         <v>3233.030303030303</v>
       </c>
-      <c r="AD16" s="185">
+      <c r="AD16" s="184">
         <f t="shared" si="5"/>
         <v>1187.0601589103292</v>
       </c>
       <c r="AE16" s="5"/>
-      <c r="AF16" s="171">
+      <c r="AF16" s="170">
         <v>4700</v>
       </c>
-      <c r="AG16" s="171">
+      <c r="AG16" s="170">
         <v>1800</v>
       </c>
-      <c r="AH16" s="172">
+      <c r="AH16" s="171">
         <v>2300</v>
       </c>
-      <c r="AI16" s="171">
+      <c r="AI16" s="170">
         <v>3500</v>
       </c>
       <c r="AM16" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="AN16" s="179">
+      <c r="AN16" s="178">
         <v>0.65947786606129399</v>
       </c>
-      <c r="AO16" s="179">
+      <c r="AO16" s="178">
         <v>0.68235651381718798</v>
       </c>
-      <c r="AP16" s="179">
+      <c r="AP16" s="178">
         <v>0.68787878787878787</v>
       </c>
     </row>
@@ -7040,42 +7069,42 @@
       <c r="W17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="AA17" s="168" t="s">
+      <c r="AA17" s="167" t="s">
         <v>134</v>
       </c>
-      <c r="AB17" s="183">
+      <c r="AB17" s="182">
         <f t="shared" si="3"/>
         <v>2251.7764955967205</v>
       </c>
-      <c r="AC17" s="185">
+      <c r="AC17" s="184">
         <f t="shared" si="4"/>
         <v>3645.7575757575755</v>
       </c>
-      <c r="AD17" s="185">
+      <c r="AD17" s="184">
         <f t="shared" si="5"/>
         <v>1318.955732122588</v>
       </c>
       <c r="AE17" s="5"/>
-      <c r="AF17" s="171">
+      <c r="AF17" s="170">
         <v>5300</v>
       </c>
-      <c r="AG17" s="171">
+      <c r="AG17" s="170">
         <v>2000</v>
       </c>
-      <c r="AH17" s="172">
+      <c r="AH17" s="171">
         <v>2600</v>
       </c>
-      <c r="AI17" s="171">
+      <c r="AI17" s="170">
         <v>4000</v>
       </c>
       <c r="AM17" s="101"/>
-      <c r="AN17" s="179">
+      <c r="AN17" s="178">
         <v>0.65947786606129399</v>
       </c>
-      <c r="AO17" s="179">
+      <c r="AO17" s="178">
         <v>0.68235651381718798</v>
       </c>
-      <c r="AP17" s="179">
+      <c r="AP17" s="178">
         <v>0.68787878787878787</v>
       </c>
     </row>
@@ -7104,76 +7133,76 @@
       <c r="O18" s="91" t="s">
         <v>119</v>
       </c>
-      <c r="P18" s="188">
+      <c r="P18" s="187">
         <f t="shared" ref="P18:P25" si="8">1-W4/$W$12</f>
         <v>0.82657317923529827</v>
       </c>
-      <c r="Q18" s="189">
+      <c r="Q18" s="188">
         <f t="shared" ref="Q18:Q24" si="9">1-W4/$W$11</f>
         <v>0.73202753715113</v>
       </c>
-      <c r="R18" s="189">
+      <c r="R18" s="188">
         <f t="shared" ref="R18:R23" si="10">1-W4/$W$10</f>
         <v>0.67174081354445081</v>
       </c>
-      <c r="S18" s="189">
+      <c r="S18" s="188">
         <f>1-W4/$W$9</f>
         <v>0.56505827081684434</v>
       </c>
-      <c r="T18" s="189">
+      <c r="T18" s="188">
         <f>1-W4/$W$8</f>
         <v>0.37746294118133139</v>
       </c>
-      <c r="U18" s="189">
+      <c r="U18" s="188">
         <f>1-W4/$W$7</f>
         <v>0.46288924705058421</v>
       </c>
-      <c r="V18" s="190">
+      <c r="V18" s="189">
         <f>1-W4/$W$6</f>
         <v>0.35059104001588781</v>
       </c>
-      <c r="W18" s="190">
+      <c r="W18" s="189">
         <f>1-W4/$W$5</f>
         <v>0.1678792793901257</v>
       </c>
-      <c r="AA18" s="168" t="s">
+      <c r="AA18" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="AB18" s="183">
+      <c r="AB18" s="182">
         <f t="shared" si="3"/>
         <v>2739.9647887323945</v>
       </c>
-      <c r="AC18" s="185">
+      <c r="AC18" s="184">
         <f t="shared" si="4"/>
         <v>4403.3907830648186</v>
       </c>
-      <c r="AD18" s="185">
+      <c r="AD18" s="184">
         <f t="shared" si="5"/>
         <v>1626.2626262626261</v>
       </c>
       <c r="AE18" s="5"/>
-      <c r="AF18" s="171">
+      <c r="AF18" s="170">
         <v>6300</v>
       </c>
-      <c r="AG18" s="171">
+      <c r="AG18" s="170">
         <v>2400</v>
       </c>
-      <c r="AH18" s="172">
+      <c r="AH18" s="171">
         <v>3200</v>
       </c>
-      <c r="AI18" s="171">
+      <c r="AI18" s="170">
         <v>4700</v>
       </c>
       <c r="AM18" s="96" t="s">
         <v>135</v>
       </c>
-      <c r="AN18" s="178">
+      <c r="AN18" s="177">
         <v>0.67760942760942755</v>
       </c>
-      <c r="AO18" s="178">
+      <c r="AO18" s="177">
         <v>0.69366197183098599</v>
       </c>
-      <c r="AP18" s="178">
+      <c r="AP18" s="177">
         <v>0.69895091794679653</v>
       </c>
     </row>
@@ -7196,73 +7225,73 @@
       <c r="O19" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="P19" s="188">
+      <c r="P19" s="187">
         <f t="shared" si="8"/>
         <v>0.79158454239957576</v>
       </c>
-      <c r="Q19" s="189">
+      <c r="Q19" s="188">
         <f t="shared" si="9"/>
         <v>0.67796443927935268</v>
       </c>
-      <c r="R19" s="189">
+      <c r="R19" s="188">
         <f t="shared" si="10"/>
         <v>0.60551494714016629</v>
       </c>
-      <c r="S19" s="189">
+      <c r="S19" s="188">
         <f>1-W5/$W$9</f>
         <v>0.47730933936559095</v>
       </c>
-      <c r="T19" s="190">
+      <c r="T19" s="189">
         <f>1-W5/$W$8</f>
         <v>0.25186689455058697</v>
       </c>
-      <c r="U19" s="190">
+      <c r="U19" s="189">
         <f>1-W5/$W$7</f>
         <v>0.35452784716650365</v>
       </c>
-      <c r="V19" s="190">
+      <c r="V19" s="189">
         <f>1-W5/$W$6</f>
         <v>0.21957362207234754</v>
       </c>
-      <c r="W19" s="188"/>
-      <c r="AA19" s="173" t="s">
+      <c r="W19" s="187"/>
+      <c r="AA19" s="172" t="s">
         <v>136</v>
       </c>
-      <c r="AB19" s="183">
+      <c r="AB19" s="182">
         <f t="shared" si="3"/>
         <v>2702.039715087416</v>
       </c>
-      <c r="AC19" s="186">
+      <c r="AC19" s="185">
         <f t="shared" si="4"/>
         <v>4397.9254406488853</v>
       </c>
-      <c r="AD19" s="186">
+      <c r="AD19" s="185">
         <f t="shared" si="5"/>
         <v>1686.5833785985876</v>
       </c>
       <c r="AE19" s="5"/>
-      <c r="AF19" s="174">
+      <c r="AF19" s="173">
         <v>7900</v>
       </c>
-      <c r="AG19" s="174">
+      <c r="AG19" s="173">
         <v>3000</v>
       </c>
-      <c r="AH19" s="175">
+      <c r="AH19" s="174">
         <v>4000</v>
       </c>
-      <c r="AI19" s="174">
+      <c r="AI19" s="173">
         <v>5900</v>
       </c>
       <c r="AM19" s="107" t="s">
         <v>136</v>
       </c>
-      <c r="AN19" s="180">
+      <c r="AN19" s="179">
         <v>0.56219445953286251</v>
       </c>
-      <c r="AO19" s="180">
+      <c r="AO19" s="179">
         <v>0.54586660910856888</v>
       </c>
-      <c r="AP19" s="180">
+      <c r="AP19" s="179">
         <v>0.55669942286694751</v>
       </c>
     </row>
@@ -7285,33 +7314,33 @@
       <c r="O20" s="101" t="s">
         <v>123</v>
       </c>
-      <c r="P20" s="189">
+      <c r="P20" s="188">
         <f t="shared" si="8"/>
         <v>0.73294667697694738</v>
       </c>
-      <c r="Q20" s="189">
+      <c r="Q20" s="188">
         <f t="shared" si="9"/>
         <v>0.58735946166276198</v>
       </c>
-      <c r="R20" s="189">
+      <c r="R20" s="188">
         <f t="shared" si="10"/>
         <v>0.49452624358065522</v>
       </c>
-      <c r="S20" s="190">
+      <c r="S20" s="189">
         <f>1-W6/$W$9</f>
         <v>0.33024987953077123</v>
       </c>
-      <c r="T20" s="190">
+      <c r="T20" s="189">
         <f>1-W6/$W$8</f>
         <v>4.1379012026721895E-2</v>
       </c>
-      <c r="U20" s="190">
+      <c r="U20" s="189">
         <f>1-W6/$W$7</f>
         <v>0.17292371056513256</v>
       </c>
-      <c r="V20" s="188"/>
-      <c r="W20" s="188"/>
-      <c r="AA20" s="163" t="s">
+      <c r="V20" s="187"/>
+      <c r="W20" s="187"/>
+      <c r="AA20" s="162" t="s">
         <v>180</v>
       </c>
     </row>
@@ -7324,30 +7353,30 @@
       <c r="O21" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="P21" s="189">
+      <c r="P21" s="188">
         <f t="shared" si="8"/>
         <v>0.67711162025267657</v>
       </c>
-      <c r="Q21" s="189">
+      <c r="Q21" s="188">
         <f t="shared" si="9"/>
         <v>0.50108527640274758</v>
       </c>
-      <c r="R21" s="189">
+      <c r="R21" s="188">
         <f t="shared" si="10"/>
         <v>0.38884264622707332</v>
       </c>
-      <c r="S21" s="190">
+      <c r="S21" s="189">
         <f>1-W7/$W$9</f>
         <v>0.19021965805976382</v>
       </c>
-      <c r="T21" s="190">
+      <c r="T21" s="189">
         <f>IF(1-W7/$W$8&lt;0,0)</f>
         <v>0</v>
       </c>
-      <c r="U21" s="188"/>
-      <c r="V21" s="188"/>
-      <c r="W21" s="188"/>
-      <c r="AA21" s="164" t="s">
+      <c r="U21" s="187"/>
+      <c r="V21" s="187"/>
+      <c r="W21" s="187"/>
+      <c r="AA21" s="163" t="s">
         <v>181</v>
       </c>
     </row>
@@ -7364,128 +7393,128 @@
       <c r="O22" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="P22" s="189">
+      <c r="P22" s="188">
         <f t="shared" si="8"/>
         <v>0.72141928210057427</v>
       </c>
-      <c r="Q22" s="189">
+      <c r="Q22" s="188">
         <f t="shared" si="9"/>
         <v>0.56954777381867572</v>
       </c>
-      <c r="R22" s="189">
+      <c r="R22" s="188">
         <f t="shared" si="10"/>
         <v>0.47270739660309302</v>
       </c>
-      <c r="S22" s="190">
+      <c r="S22" s="189">
         <f>1-W8/$W$9</f>
         <v>0.30134001980780933</v>
       </c>
-      <c r="T22" s="188"/>
-      <c r="U22" s="188"/>
-      <c r="V22" s="188"/>
-      <c r="W22" s="188"/>
+      <c r="T22" s="187"/>
+      <c r="U22" s="187"/>
+      <c r="V22" s="187"/>
+      <c r="W22" s="187"/>
     </row>
     <row r="23" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>193</v>
       </c>
-      <c r="F23" s="144">
+      <c r="F23" s="143">
         <f>F18/$D$14</f>
         <v>0.12047183066805627</v>
       </c>
-      <c r="G23" s="144">
+      <c r="G23" s="143">
         <f>G18/$E$14</f>
         <v>0.14269122682268837</v>
       </c>
-      <c r="H23" s="144">
+      <c r="H23" s="143">
         <f>H18/$F$14</f>
         <v>0.24586456547937455</v>
       </c>
       <c r="O23" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="P23" s="189">
+      <c r="P23" s="188">
         <f t="shared" si="8"/>
         <v>0.60126424040662463</v>
       </c>
-      <c r="Q23" s="189">
+      <c r="Q23" s="188">
         <f t="shared" si="9"/>
         <v>0.38388881804434616</v>
       </c>
-      <c r="R23" s="190">
+      <c r="R23" s="189">
         <f t="shared" si="10"/>
         <v>0.24528008137541124</v>
       </c>
-      <c r="S23" s="188"/>
-      <c r="T23" s="188"/>
-      <c r="U23" s="188"/>
-      <c r="V23" s="188"/>
-      <c r="W23" s="188"/>
+      <c r="S23" s="187"/>
+      <c r="T23" s="187"/>
+      <c r="U23" s="187"/>
+      <c r="V23" s="187"/>
+      <c r="W23" s="187"/>
     </row>
     <row r="24" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>194</v>
       </c>
-      <c r="F24" s="144">
+      <c r="F24" s="143">
         <f t="shared" ref="F24:F25" si="13">F19/$D$14</f>
         <v>0.36817497729041837</v>
       </c>
-      <c r="G24" s="144">
+      <c r="G24" s="143">
         <f t="shared" ref="G24:G25" si="14">G19/$E$14</f>
         <v>0.34691968530979972</v>
       </c>
-      <c r="H24" s="144">
+      <c r="H24" s="143">
         <f t="shared" ref="H24:H25" si="15">H19/$F$14</f>
         <v>0.28484101080348528</v>
       </c>
       <c r="O24" s="101" t="s">
         <v>133</v>
       </c>
-      <c r="P24" s="189">
+      <c r="P24" s="188">
         <f t="shared" si="8"/>
         <v>0.47167717486503269</v>
       </c>
-      <c r="Q24" s="190">
+      <c r="Q24" s="189">
         <f t="shared" si="9"/>
         <v>0.18365586126511313</v>
       </c>
-      <c r="R24" s="188"/>
-      <c r="S24" s="188"/>
-      <c r="T24" s="188"/>
-      <c r="U24" s="188"/>
-      <c r="V24" s="188"/>
-      <c r="W24" s="188"/>
+      <c r="R24" s="187"/>
+      <c r="S24" s="187"/>
+      <c r="T24" s="187"/>
+      <c r="U24" s="187"/>
+      <c r="V24" s="187"/>
+      <c r="W24" s="187"/>
     </row>
     <row r="25" spans="1:42" ht="15" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>195</v>
       </c>
-      <c r="F25" s="144">
+      <c r="F25" s="143">
         <f t="shared" si="13"/>
         <v>0.51135319204152541</v>
       </c>
-      <c r="G25" s="144">
+      <c r="G25" s="143">
         <f t="shared" si="14"/>
         <v>0.5103890878675118</v>
       </c>
-      <c r="H25" s="144">
+      <c r="H25" s="143">
         <f t="shared" si="15"/>
         <v>0.46929442371714014</v>
       </c>
       <c r="O25" s="96" t="s">
         <v>135</v>
       </c>
-      <c r="P25" s="190">
+      <c r="P25" s="189">
         <f t="shared" si="8"/>
         <v>0.3528184988824381</v>
       </c>
-      <c r="Q25" s="190"/>
-      <c r="R25" s="188"/>
-      <c r="S25" s="188"/>
-      <c r="T25" s="188"/>
-      <c r="U25" s="188"/>
-      <c r="V25" s="188"/>
-      <c r="W25" s="188"/>
+      <c r="Q25" s="189"/>
+      <c r="R25" s="187"/>
+      <c r="S25" s="187"/>
+      <c r="T25" s="187"/>
+      <c r="U25" s="187"/>
+      <c r="V25" s="187"/>
+      <c r="W25" s="187"/>
     </row>
     <row r="26" spans="1:42" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:42" x14ac:dyDescent="0.2">
@@ -7501,40 +7530,40 @@
       <c r="A29" s="117" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="211" t="s">
+      <c r="C29" s="210" t="s">
         <v>163</v>
       </c>
-      <c r="D29" s="212"/>
-      <c r="E29" s="212"/>
-      <c r="F29" s="212"/>
-      <c r="G29" s="213"/>
-      <c r="H29" s="211" t="s">
+      <c r="D29" s="211"/>
+      <c r="E29" s="211"/>
+      <c r="F29" s="211"/>
+      <c r="G29" s="212"/>
+      <c r="H29" s="210" t="s">
         <v>182</v>
       </c>
-      <c r="I29" s="212"/>
-      <c r="J29" s="212"/>
-      <c r="K29" s="212"/>
-      <c r="L29" s="213"/>
-      <c r="M29" s="205" t="s">
+      <c r="I29" s="211"/>
+      <c r="J29" s="211"/>
+      <c r="K29" s="211"/>
+      <c r="L29" s="212"/>
+      <c r="M29" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="N29" s="206"/>
-      <c r="O29" s="206"/>
-      <c r="P29" s="205" t="s">
+      <c r="N29" s="205"/>
+      <c r="O29" s="205"/>
+      <c r="P29" s="204" t="s">
         <v>191</v>
       </c>
-      <c r="Q29" s="206"/>
-      <c r="R29" s="206"/>
-      <c r="S29" s="205" t="s">
+      <c r="Q29" s="205"/>
+      <c r="R29" s="205"/>
+      <c r="S29" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="T29" s="206"/>
-      <c r="U29" s="206"/>
-      <c r="V29" s="205" t="s">
+      <c r="T29" s="205"/>
+      <c r="U29" s="205"/>
+      <c r="V29" s="204" t="s">
         <v>192</v>
       </c>
-      <c r="W29" s="206"/>
-      <c r="X29" s="206"/>
+      <c r="W29" s="205"/>
+      <c r="X29" s="205"/>
     </row>
     <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="116" t="s">
@@ -7602,7 +7631,7 @@
       <c r="X30" s="129" t="s">
         <v>106</v>
       </c>
-      <c r="AA30" s="182" t="s">
+      <c r="AA30" s="181" t="s">
         <v>182</v>
       </c>
     </row>
@@ -7722,7 +7751,7 @@
       <c r="S33" s="126"/>
       <c r="T33" s="126"/>
       <c r="U33" s="126"/>
-      <c r="AA33" s="182" t="s">
+      <c r="AA33" s="181" t="s">
         <v>213</v>
       </c>
     </row>
@@ -9352,29 +9381,29 @@
       <c r="C60" t="s">
         <v>183</v>
       </c>
-      <c r="S60" s="137">
-        <f>SUM(S38,S41,S44,S48,S53,S57)</f>
-        <v>20563.0239417189</v>
-      </c>
-      <c r="T60" s="137">
-        <f t="shared" ref="T60:W60" si="58">SUM(T38,T41,T44,T48,T53,T57)</f>
-        <v>22259.387557085229</v>
-      </c>
-      <c r="U60" s="137">
-        <f t="shared" si="58"/>
-        <v>15982.779351113084</v>
-      </c>
-      <c r="V60" s="138">
-        <f t="shared" si="58"/>
-        <v>0.41971707986779133</v>
-      </c>
-      <c r="W60" s="138">
-        <f t="shared" si="58"/>
-        <v>0.42725634048359507</v>
-      </c>
-      <c r="X60" s="138">
-        <f>SUM(X38,X41,X44,X48,X53,X57)</f>
-        <v>0.36362775898499861</v>
+      <c r="S60" s="213" cm="1">
+        <f t="array" ref="S60">S38+AVERAGE(S40:S41)+AVERAGE(S43:S45)+AVERAGE(S47:S50+AVERAGE(S53:S56))</f>
+        <v>22294.679797673529</v>
+      </c>
+      <c r="T60" s="213" cm="1">
+        <f t="array" ref="T60">T38+AVERAGE(T40:T41)+AVERAGE(T43:T45)+AVERAGE(T47:T50+AVERAGE(T53:T56))</f>
+        <v>24114.356797661487</v>
+      </c>
+      <c r="U60" s="213" cm="1">
+        <f t="array" ref="U60">U38+AVERAGE(U40:U41)+AVERAGE(U43:U45)+AVERAGE(U47:U50+AVERAGE(U53:U56))</f>
+        <v>17266.169771719473</v>
+      </c>
+      <c r="V60" s="137" cm="1">
+        <f t="array" ref="V60">V38+AVERAGE(V40:V41)+AVERAGE(V43:V45)+AVERAGE(V47:V50+AVERAGE(V53:V56))</f>
+        <v>0.44109160694603122</v>
+      </c>
+      <c r="W60" s="137" cm="1">
+        <f t="array" ref="W60">W38+AVERAGE(W40:W41)+AVERAGE(W43:W45)+AVERAGE(W47:W50+AVERAGE(W53:W56))</f>
+        <v>0.43814428681539097</v>
+      </c>
+      <c r="X60" s="137" cm="1">
+        <f t="array" ref="X60">X38+AVERAGE(X40:X41)+AVERAGE(X43:X45)+AVERAGE(X47:X50+AVERAGE(X53:X56))</f>
+        <v>0.37835986642564029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pre-measure retrofit data in RSD-Retrofit
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B52CE5-5141-42B1-BE25-4CF95BFB9EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D795C4F-A041-4569-A64D-44DA8DA22072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -2358,6 +2358,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="14" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="20" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="14" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="44" fillId="20" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2427,7 +2428,6 @@
     <xf numFmtId="0" fontId="43" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="44" fillId="20" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - Colore 2" xfId="10" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
@@ -3998,14 +3998,14 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="191" t="s">
+      <c r="A17" s="192" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="191"/>
-      <c r="C17" s="191"/>
-      <c r="D17" s="191"/>
-      <c r="E17" s="191"/>
-      <c r="F17" s="191"/>
+      <c r="B17" s="192"/>
+      <c r="C17" s="192"/>
+      <c r="D17" s="192"/>
+      <c r="E17" s="192"/>
+      <c r="F17" s="192"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
@@ -4043,13 +4043,13 @@
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="192" t="s">
+      <c r="B20" s="193" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="192"/>
-      <c r="D20" s="192"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
+      <c r="C20" s="193"/>
+      <c r="D20" s="193"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="14"/>
@@ -4063,13 +4063,13 @@
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="193" t="s">
+      <c r="B21" s="194" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="193"/>
-      <c r="D21" s="193"/>
-      <c r="E21" s="193"/>
-      <c r="F21" s="193"/>
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="194"/>
+      <c r="F21" s="194"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="14"/>
@@ -4083,13 +4083,13 @@
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="193" t="s">
+      <c r="B22" s="194" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="193"/>
-      <c r="D22" s="193"/>
-      <c r="E22" s="193"/>
-      <c r="F22" s="193"/>
+      <c r="C22" s="194"/>
+      <c r="D22" s="194"/>
+      <c r="E22" s="194"/>
+      <c r="F22" s="194"/>
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -4118,22 +4118,22 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="194"/>
-      <c r="B25" s="194"/>
-      <c r="C25" s="194"/>
-      <c r="D25" s="194"/>
-      <c r="E25" s="194"/>
-      <c r="F25" s="194"/>
+      <c r="A25" s="195"/>
+      <c r="B25" s="195"/>
+      <c r="C25" s="195"/>
+      <c r="D25" s="195"/>
+      <c r="E25" s="195"/>
+      <c r="F25" s="195"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="190"/>
-      <c r="B26" s="190"/>
-      <c r="C26" s="190"/>
-      <c r="D26" s="190"/>
-      <c r="E26" s="190"/>
-      <c r="F26" s="190"/>
+      <c r="A26" s="191"/>
+      <c r="B26" s="191"/>
+      <c r="C26" s="191"/>
+      <c r="D26" s="191"/>
+      <c r="E26" s="191"/>
+      <c r="F26" s="191"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
@@ -4320,17 +4320,17 @@
   <sheetData>
     <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+      <c r="E2" s="198"/>
       <c r="F2" s="147"/>
-      <c r="H2" s="195" t="s">
+      <c r="H2" s="196" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="197"/>
+      <c r="I2" s="198"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -4640,10 +4640,10 @@
         <v>80</v>
       </c>
       <c r="F15" s="149"/>
-      <c r="H15" s="195" t="s">
+      <c r="H15" s="196" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="197"/>
+      <c r="I15" s="198"/>
     </row>
     <row r="16" spans="2:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
@@ -4717,12 +4717,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="198" t="s">
+      <c r="B20" s="199" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="199"/>
-      <c r="D20" s="199"/>
-      <c r="E20" s="200"/>
+      <c r="C20" s="200"/>
+      <c r="D20" s="200"/>
+      <c r="E20" s="201"/>
       <c r="F20" s="150"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4933,17 +4933,17 @@
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="195" t="s">
+      <c r="B38" s="196" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="196"/>
-      <c r="D38" s="196"/>
-      <c r="E38" s="197"/>
+      <c r="C38" s="197"/>
+      <c r="D38" s="197"/>
+      <c r="E38" s="198"/>
       <c r="F38" s="147"/>
-      <c r="H38" s="201" t="s">
+      <c r="H38" s="202" t="s">
         <v>56</v>
       </c>
-      <c r="I38" s="202"/>
+      <c r="I38" s="203"/>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="61" t="s">
@@ -5049,8 +5049,8 @@
   </sheetPr>
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5065,7 +5065,9 @@
     <col min="13" max="14" width="9.140625" style="80"/>
     <col min="15" max="15" width="9.5703125" style="80" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="80"/>
-    <col min="17" max="21" width="11.140625" style="80" customWidth="1"/>
+    <col min="17" max="18" width="11.140625" style="80" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" style="80" customWidth="1"/>
+    <col min="20" max="21" width="11.140625" style="80" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="80"/>
   </cols>
   <sheetData>
@@ -5148,10 +5150,10 @@
       <c r="S5" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="T5" s="203" t="s">
+      <c r="T5" s="204" t="s">
         <v>114</v>
       </c>
-      <c r="U5" s="203"/>
+      <c r="U5" s="204"/>
     </row>
     <row r="6" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
@@ -5247,7 +5249,7 @@
       </c>
       <c r="N7" s="75">
         <f>U7</f>
-        <v>3.4901289446216035E-3</v>
+        <v>3.0320495206400178E-3</v>
       </c>
       <c r="O7" s="139">
         <f>Data!U59/1000</f>
@@ -5260,7 +5262,7 @@
         <v>109</v>
       </c>
       <c r="S7" s="80">
-        <v>1.6E-2</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="T7" s="141">
         <f>Data!X59</f>
@@ -5268,7 +5270,7 @@
       </c>
       <c r="U7" s="80">
         <f>S7*T7</f>
-        <v>3.4901289446216035E-3</v>
+        <v>3.0320495206400178E-3</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5311,7 +5313,7 @@
       </c>
       <c r="N8" s="83">
         <f t="shared" ref="N8:N12" si="4">U8</f>
-        <v>6.053757862810245E-3</v>
+        <v>5.2592021433163997E-3</v>
       </c>
       <c r="O8" s="140">
         <f>Data!U60/1000</f>
@@ -5324,7 +5326,7 @@
         <v>110</v>
       </c>
       <c r="S8" s="81">
-        <v>1.6E-2</v>
+        <v>1.3899999999999999E-2</v>
       </c>
       <c r="T8" s="142">
         <f>Data!X60</f>
@@ -5332,7 +5334,7 @@
       </c>
       <c r="U8" s="81">
         <f t="shared" ref="U8:U12" si="5">S8*T8</f>
-        <v>6.053757862810245E-3</v>
+        <v>5.2592021433163997E-3</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5375,7 +5377,7 @@
       </c>
       <c r="N9" s="75">
         <f t="shared" si="4"/>
-        <v>5.4263583940724319E-3</v>
+        <v>5.7087710985966478E-3</v>
       </c>
       <c r="O9" s="139">
         <f>Data!S59/1000</f>
@@ -5388,7 +5390,7 @@
         <v>109</v>
       </c>
       <c r="S9" s="80">
-        <v>2.69E-2</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="T9" s="141">
         <f>Data!V59</f>
@@ -5396,7 +5398,7 @@
       </c>
       <c r="U9" s="80">
         <f t="shared" si="5"/>
-        <v>5.4263583940724319E-3</v>
+        <v>5.7087710985966478E-3</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5439,7 +5441,7 @@
       </c>
       <c r="N10" s="83">
         <f t="shared" si="4"/>
-        <v>1.186536422684824E-2</v>
+        <v>1.2482892476572683E-2</v>
       </c>
       <c r="O10" s="140">
         <f>Data!S60/1000</f>
@@ -5452,7 +5454,7 @@
         <v>110</v>
       </c>
       <c r="S10" s="81">
-        <v>2.69E-2</v>
+        <v>2.8299999999999999E-2</v>
       </c>
       <c r="T10" s="142">
         <f>Data!V60</f>
@@ -5460,7 +5462,7 @@
       </c>
       <c r="U10" s="81">
         <f t="shared" si="5"/>
-        <v>1.186536422684824E-2</v>
+        <v>1.2482892476572683E-2</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5503,7 +5505,7 @@
       </c>
       <c r="N11" s="75">
         <f t="shared" si="4"/>
-        <v>9.5809185652412903E-3</v>
+        <v>1.0380995272150794E-2</v>
       </c>
       <c r="O11" s="139">
         <f>Data!T59/1000</f>
@@ -5516,7 +5518,7 @@
         <v>109</v>
       </c>
       <c r="S11" s="80">
-        <v>4.7899999999999998E-2</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="T11" s="141">
         <f>Data!W59</f>
@@ -5524,7 +5526,7 @@
       </c>
       <c r="U11" s="80">
         <f t="shared" si="5"/>
-        <v>9.5809185652412903E-3</v>
+        <v>1.0380995272150794E-2</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.2">
@@ -5567,7 +5569,7 @@
       </c>
       <c r="N12" s="83">
         <f t="shared" si="4"/>
-        <v>2.0987111338457227E-2</v>
+        <v>2.2739688485718793E-2</v>
       </c>
       <c r="O12" s="140">
         <f>Data!T60/1000</f>
@@ -5580,7 +5582,7 @@
         <v>110</v>
       </c>
       <c r="S12" s="81">
-        <v>4.7899999999999998E-2</v>
+        <v>5.1900000000000002E-2</v>
       </c>
       <c r="T12" s="142">
         <f>Data!W60</f>
@@ -5588,7 +5590,7 @@
       </c>
       <c r="U12" s="81">
         <f t="shared" si="5"/>
-        <v>2.0987111338457227E-2</v>
+        <v>2.2739688485718793E-2</v>
       </c>
     </row>
     <row r="19" spans="22:26" x14ac:dyDescent="0.2">
@@ -5832,7 +5834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A6DB4B-6EBE-42F5-800F-C9AB0144B3BB}">
   <dimension ref="A1:AP60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
@@ -5863,33 +5865,33 @@
   <sheetData>
     <row r="1" spans="3:42" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L2" s="207" t="s">
+      <c r="L2" s="208" t="s">
         <v>175</v>
       </c>
-      <c r="M2" s="208"/>
-      <c r="N2" s="209"/>
-      <c r="O2" s="207" t="s">
+      <c r="M2" s="209"/>
+      <c r="N2" s="210"/>
+      <c r="O2" s="208" t="s">
         <v>176</v>
       </c>
-      <c r="P2" s="208"/>
-      <c r="Q2" s="209"/>
-      <c r="R2" s="207" t="s">
+      <c r="P2" s="209"/>
+      <c r="Q2" s="210"/>
+      <c r="R2" s="208" t="s">
         <v>186</v>
       </c>
-      <c r="S2" s="208"/>
-      <c r="T2" s="209"/>
+      <c r="S2" s="209"/>
+      <c r="T2" s="210"/>
       <c r="AD2" s="118" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="3" spans="3:42" ht="21.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="206" t="s">
+      <c r="C3" s="207" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="206"/>
-      <c r="E3" s="206"/>
-      <c r="F3" s="206"/>
-      <c r="G3" s="206"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
       <c r="L3" s="88" t="s">
         <v>165</v>
       </c>
@@ -7530,40 +7532,40 @@
       <c r="A29" s="117" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="210" t="s">
+      <c r="C29" s="211" t="s">
         <v>163</v>
       </c>
-      <c r="D29" s="211"/>
-      <c r="E29" s="211"/>
-      <c r="F29" s="211"/>
-      <c r="G29" s="212"/>
-      <c r="H29" s="210" t="s">
+      <c r="D29" s="212"/>
+      <c r="E29" s="212"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="213"/>
+      <c r="H29" s="211" t="s">
         <v>182</v>
       </c>
-      <c r="I29" s="211"/>
-      <c r="J29" s="211"/>
-      <c r="K29" s="211"/>
-      <c r="L29" s="212"/>
-      <c r="M29" s="204" t="s">
+      <c r="I29" s="212"/>
+      <c r="J29" s="212"/>
+      <c r="K29" s="212"/>
+      <c r="L29" s="213"/>
+      <c r="M29" s="205" t="s">
         <v>190</v>
       </c>
-      <c r="N29" s="205"/>
-      <c r="O29" s="205"/>
-      <c r="P29" s="204" t="s">
+      <c r="N29" s="206"/>
+      <c r="O29" s="206"/>
+      <c r="P29" s="205" t="s">
         <v>191</v>
       </c>
-      <c r="Q29" s="205"/>
-      <c r="R29" s="205"/>
-      <c r="S29" s="204" t="s">
+      <c r="Q29" s="206"/>
+      <c r="R29" s="206"/>
+      <c r="S29" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="T29" s="205"/>
-      <c r="U29" s="205"/>
-      <c r="V29" s="204" t="s">
+      <c r="T29" s="206"/>
+      <c r="U29" s="206"/>
+      <c r="V29" s="205" t="s">
         <v>192</v>
       </c>
-      <c r="W29" s="205"/>
-      <c r="X29" s="205"/>
+      <c r="W29" s="206"/>
+      <c r="X29" s="206"/>
     </row>
     <row r="30" spans="1:42" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="116" t="s">
@@ -9381,15 +9383,15 @@
       <c r="C60" t="s">
         <v>183</v>
       </c>
-      <c r="S60" s="213" cm="1">
+      <c r="S60" s="190" cm="1">
         <f t="array" ref="S60">S38+AVERAGE(S40:S41)+AVERAGE(S43:S45)+AVERAGE(S47:S50+AVERAGE(S53:S56))</f>
         <v>22294.679797673529</v>
       </c>
-      <c r="T60" s="213" cm="1">
+      <c r="T60" s="190" cm="1">
         <f t="array" ref="T60">T38+AVERAGE(T40:T41)+AVERAGE(T43:T45)+AVERAGE(T47:T50+AVERAGE(T53:T56))</f>
         <v>24114.356797661487</v>
       </c>
-      <c r="U60" s="213" cm="1">
+      <c r="U60" s="190" cm="1">
         <f t="array" ref="U60">U38+AVERAGE(U40:U41)+AVERAGE(U43:U45)+AVERAGE(U47:U50+AVERAGE(U53:U56))</f>
         <v>17266.169771719473</v>
       </c>

</xml_diff>

<commit_message>
Put Retrofits back, slight increase in Electricity Resistance Heater
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF43923A-3A80-40CC-A503-4F99928272C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ECDE56-B4DA-4CB6-BC17-B7D2FBF65901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2760" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{61E3DBC4-3D48-40CE-BDD5-C17192DCDA09}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="34" r:id="rId1"/>
@@ -1891,7 +1891,7 @@
     <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2427,9 +2427,6 @@
     </xf>
     <xf numFmtId="0" fontId="43" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -5053,7 +5050,7 @@
   <dimension ref="A1:Z50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5074,18 +5071,18 @@
     <col min="22" max="16384" width="9.140625" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="72" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="73"/>
     </row>
-    <row r="2" spans="1:23" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="s">
         <v>21</v>
       </c>
@@ -5100,7 +5097,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
@@ -5158,7 +5155,7 @@
       </c>
       <c r="U5" s="204"/>
     </row>
-    <row r="6" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="78" t="s">
         <v>63</v>
       </c>
@@ -5212,7 +5209,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="75" t="s">
         <v>30</v>
       </c>
@@ -5252,7 +5249,7 @@
       </c>
       <c r="N7" s="75">
         <f>U7</f>
-        <v>4.8649999999999995E-3</v>
+        <v>3.0320495206400178E-3</v>
       </c>
       <c r="O7" s="139">
         <f>Data!U59/1000</f>
@@ -5268,18 +5265,15 @@
         <v>1.3899999999999999E-2</v>
       </c>
       <c r="T7" s="141">
-        <v>0.35</v>
+        <f>Data!X59</f>
+        <v>0.21813305903885022</v>
       </c>
       <c r="U7" s="80">
         <f>S7*T7</f>
-        <v>4.8649999999999995E-3</v>
-      </c>
-      <c r="W7" s="214">
-        <f>Data!X59</f>
-        <v>0.21813305903885022</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+        <v>3.0320495206400178E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="83" t="s">
         <v>30</v>
       </c>
@@ -5319,7 +5313,7 @@
       </c>
       <c r="N8" s="83">
         <f>U8</f>
-        <v>9.0349999999999996E-3</v>
+        <v>5.2592021433163997E-3</v>
       </c>
       <c r="O8" s="140">
         <f>Data!U60/1000</f>
@@ -5334,19 +5328,16 @@
       <c r="S8" s="81">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="T8" s="142">
-        <v>0.65</v>
+      <c r="T8" s="141">
+        <f>Data!X60</f>
+        <v>0.37835986642564029</v>
       </c>
       <c r="U8" s="81">
         <f t="shared" ref="U8:U12" si="4">S8*T8</f>
-        <v>9.0349999999999996E-3</v>
-      </c>
-      <c r="W8" s="214">
-        <f>Data!X60</f>
-        <v>0.37835986642564029</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+        <v>5.2592021433163997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="75" t="s">
         <v>30</v>
       </c>
@@ -5385,8 +5376,8 @@
         <v>50</v>
       </c>
       <c r="N9" s="75">
-        <f t="shared" ref="N8:N12" si="5">U9</f>
-        <v>9.9049999999999989E-3</v>
+        <f t="shared" ref="N9:N12" si="5">U9</f>
+        <v>5.7087710985966478E-3</v>
       </c>
       <c r="O9" s="139">
         <f>Data!S59/1000</f>
@@ -5402,18 +5393,15 @@
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="T9" s="141">
-        <v>0.35</v>
+        <f>Data!V59</f>
+        <v>0.20172336037443986</v>
       </c>
       <c r="U9" s="80">
         <f t="shared" si="4"/>
-        <v>9.9049999999999989E-3</v>
-      </c>
-      <c r="W9" s="214">
-        <f>Data!V59</f>
-        <v>0.20172336037443986</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+        <v>5.7087710985966478E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="83" t="s">
         <v>30</v>
       </c>
@@ -5453,7 +5441,7 @@
       </c>
       <c r="N10" s="83">
         <f t="shared" si="5"/>
-        <v>1.9809999999999998E-2</v>
+        <v>1.2482892476572683E-2</v>
       </c>
       <c r="O10" s="140">
         <f>Data!S60/1000</f>
@@ -5469,18 +5457,15 @@
         <v>2.8299999999999999E-2</v>
       </c>
       <c r="T10" s="142">
-        <v>0.7</v>
+        <f>Data!V60</f>
+        <v>0.44109160694603122</v>
       </c>
       <c r="U10" s="81">
         <f t="shared" si="4"/>
-        <v>1.9809999999999998E-2</v>
-      </c>
-      <c r="W10" s="214">
-        <f>Data!V60</f>
-        <v>0.44109160694603122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+        <v>1.2482892476572683E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="75" t="s">
         <v>30</v>
       </c>
@@ -5520,7 +5505,7 @@
       </c>
       <c r="N11" s="75">
         <f t="shared" si="5"/>
-        <v>1.8165000000000001E-2</v>
+        <v>1.0380995272150794E-2</v>
       </c>
       <c r="O11" s="139">
         <f>Data!T59/1000</f>
@@ -5536,18 +5521,15 @@
         <v>5.1900000000000002E-2</v>
       </c>
       <c r="T11" s="141">
-        <v>0.35</v>
+        <f>Data!W59</f>
+        <v>0.2000191767273756</v>
       </c>
       <c r="U11" s="80">
         <f>S11*T11</f>
-        <v>1.8165000000000001E-2</v>
-      </c>
-      <c r="W11" s="214">
-        <f>Data!W59</f>
-        <v>0.2000191767273756</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+        <v>1.0380995272150794E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="83" t="s">
         <v>30</v>
       </c>
@@ -5587,7 +5569,7 @@
       </c>
       <c r="N12" s="83">
         <f t="shared" si="5"/>
-        <v>3.6330000000000001E-2</v>
+        <v>2.2739688485718793E-2</v>
       </c>
       <c r="O12" s="140">
         <f>Data!T60/1000</f>
@@ -5602,16 +5584,13 @@
       <c r="S12" s="81">
         <v>5.1900000000000002E-2</v>
       </c>
-      <c r="T12" s="142">
-        <v>0.7</v>
+      <c r="T12" s="141">
+        <f>Data!W60</f>
+        <v>0.43814428681539097</v>
       </c>
       <c r="U12" s="81">
         <f t="shared" si="4"/>
-        <v>3.6330000000000001E-2</v>
-      </c>
-      <c r="W12" s="214">
-        <f>Data!W60</f>
-        <v>0.43814428681539097</v>
+        <v>2.2739688485718793E-2</v>
       </c>
     </row>
     <row r="19" spans="22:26" x14ac:dyDescent="0.2">

</xml_diff>